<commit_message>
fixed the emergency manoeuvre
</commit_message>
<xml_diff>
--- a/Simulations/Results/berthing_60s_act/berthing_60s_act.xlsx
+++ b/Simulations/Results/berthing_60s_act/berthing_60s_act.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="138">
   <si>
     <t>id</t>
   </si>
@@ -253,6 +253,180 @@
   </si>
   <si>
     <t>delta_rhodot (m/s)</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>dr (m)</t>
+  </si>
+  <si>
+    <t>dtheta (m)</t>
+  </si>
+  <si>
+    <t>dh (m)</t>
+  </si>
+  <si>
+    <t>dv_r (m/s)</t>
+  </si>
+  <si>
+    <t>dv_theta (m/s)</t>
+  </si>
+  <si>
+    <t>dv_h (m/s)</t>
+  </si>
+  <si>
+    <t>delta_rho (m)</t>
+  </si>
+  <si>
+    <t>delta_rhodot (m/s)</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>dr (m)</t>
+  </si>
+  <si>
+    <t>dtheta (m)</t>
+  </si>
+  <si>
+    <t>dh (m)</t>
+  </si>
+  <si>
+    <t>dv_r (m/s)</t>
+  </si>
+  <si>
+    <t>dv_theta (m/s)</t>
+  </si>
+  <si>
+    <t>dv_h (m/s)</t>
+  </si>
+  <si>
+    <t>delta_rho (m)</t>
+  </si>
+  <si>
+    <t>delta_rhodot (m/s)</t>
+  </si>
+  <si>
+    <t>omega_ef (rad/s)</t>
+  </si>
+  <si>
+    <t>angle_e (deg)</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>dr (m)</t>
+  </si>
+  <si>
+    <t>dtheta (m)</t>
+  </si>
+  <si>
+    <t>dh (m)</t>
+  </si>
+  <si>
+    <t>dv_r (m/s)</t>
+  </si>
+  <si>
+    <t>dv_theta (m/s)</t>
+  </si>
+  <si>
+    <t>dv_h (m/s)</t>
+  </si>
+  <si>
+    <t>delta_rho (m)</t>
+  </si>
+  <si>
+    <t>delta_rhodot (m/s)</t>
+  </si>
+  <si>
+    <t>omega_ef (rad/s)</t>
+  </si>
+  <si>
+    <t>angle_e (deg)</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>dr (m)</t>
+  </si>
+  <si>
+    <t>dtheta (m)</t>
+  </si>
+  <si>
+    <t>dh (m)</t>
+  </si>
+  <si>
+    <t>dv_r (m/s)</t>
+  </si>
+  <si>
+    <t>dv_theta (m/s)</t>
+  </si>
+  <si>
+    <t>dv_h (m/s)</t>
+  </si>
+  <si>
+    <t>delta_rho (m)</t>
+  </si>
+  <si>
+    <t>delta_rhodot (m/s)</t>
+  </si>
+  <si>
+    <t>omega_ef (rad/s)</t>
+  </si>
+  <si>
+    <t>angle_e (deg)</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>dr (m)</t>
+  </si>
+  <si>
+    <t>dtheta (m)</t>
+  </si>
+  <si>
+    <t>dh (m)</t>
+  </si>
+  <si>
+    <t>dv_r (m/s)</t>
+  </si>
+  <si>
+    <t>dv_theta (m/s)</t>
+  </si>
+  <si>
+    <t>dv_h (m/s)</t>
+  </si>
+  <si>
+    <t>delta_rho (m)</t>
+  </si>
+  <si>
+    <t>delta_rhodot (m/s)</t>
+  </si>
+  <si>
+    <t>omega_ef (rad/s)</t>
+  </si>
+  <si>
+    <t>angle_e (deg)</t>
   </si>
 </sst>
 </file>
@@ -298,7 +472,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J101"/>
+  <dimension ref="A1:L101"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.15625" customWidth="true"/>
@@ -311,38 +485,46 @@
     <col min="8" max="8" width="16.046875" customWidth="true"/>
     <col min="9" max="9" width="14.7109375" customWidth="true"/>
     <col min="10" max="10" width="16.48828125" customWidth="true"/>
+    <col min="11" max="11" width="15.37890625" customWidth="true"/>
+    <col min="12" max="12" width="15.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>70</v>
+        <v>126</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>71</v>
+        <v>127</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>72</v>
+        <v>128</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>73</v>
+        <v>129</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>74</v>
+        <v>130</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>75</v>
+        <v>131</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>76</v>
+        <v>132</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>77</v>
+        <v>133</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>78</v>
+        <v>134</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>79</v>
+        <v>135</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="2">
@@ -375,6 +557,12 @@
       </c>
       <c r="J2" s="0">
         <v>4.5573984827654708e-05</v>
+      </c>
+      <c r="K2" s="0">
+        <v>4.7706807848783269e-10</v>
+      </c>
+      <c r="L2" s="0">
+        <v>0.001168793203355593</v>
       </c>
     </row>
     <row r="3">
@@ -408,6 +596,12 @@
       <c r="J3" s="0">
         <v>3.8914302331147117e-05</v>
       </c>
+      <c r="K3" s="0">
+        <v>2.8701331050082988e-10</v>
+      </c>
+      <c r="L3" s="0">
+        <v>0.00023150090311049355</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
@@ -440,6 +634,12 @@
       <c r="J4" s="0">
         <v>2.4109815999077132e-05</v>
       </c>
+      <c r="K4" s="0">
+        <v>3.7052458372844564e-10</v>
+      </c>
+      <c r="L4" s="0">
+        <v>0.0022230175729369707</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
@@ -472,6 +672,12 @@
       <c r="J5" s="0">
         <v>4.9271715417006557e-05</v>
       </c>
+      <c r="K5" s="0">
+        <v>2.1857108941018615e-10</v>
+      </c>
+      <c r="L5" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
@@ -504,6 +710,12 @@
       <c r="J6" s="0">
         <v>1.3598451726191262e-05</v>
       </c>
+      <c r="K6" s="0">
+        <v>2.5162175920485892e-10</v>
+      </c>
+      <c r="L6" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
@@ -536,6 +748,12 @@
       <c r="J7" s="0">
         <v>3.8229393933635504e-05</v>
       </c>
+      <c r="K7" s="0">
+        <v>1.3283024370886434e-11</v>
+      </c>
+      <c r="L7" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
@@ -568,6 +786,12 @@
       <c r="J8" s="0">
         <v>4.1302097661642674e-05</v>
       </c>
+      <c r="K8" s="0">
+        <v>1.2894290806585825e-10</v>
+      </c>
+      <c r="L8" s="0">
+        <v>0.00086053086860947805</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
@@ -600,6 +824,12 @@
       <c r="J9" s="0">
         <v>2.6016990074176194e-05</v>
       </c>
+      <c r="K9" s="0">
+        <v>3.1113419813451818e-10</v>
+      </c>
+      <c r="L9" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
@@ -632,6 +862,12 @@
       <c r="J10" s="0">
         <v>7.2067697294210626e-05</v>
       </c>
+      <c r="K10" s="0">
+        <v>5.2154416163673955e-11</v>
+      </c>
+      <c r="L10" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
@@ -664,6 +900,12 @@
       <c r="J11" s="0">
         <v>5.3911807722167254e-05</v>
       </c>
+      <c r="K11" s="0">
+        <v>1.5656765998037746e-09</v>
+      </c>
+      <c r="L11" s="0">
+        <v>0.0004484534146647257</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
@@ -696,6 +938,12 @@
       <c r="J12" s="0">
         <v>2.0098896056833194e-05</v>
       </c>
+      <c r="K12" s="0">
+        <v>5.2338878242506022e-10</v>
+      </c>
+      <c r="L12" s="0">
+        <v>0.0018188191544244385</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
@@ -728,6 +976,12 @@
       <c r="J13" s="0">
         <v>7.9688308804253114e-06</v>
       </c>
+      <c r="K13" s="0">
+        <v>1.7745344490065358e-10</v>
+      </c>
+      <c r="L13" s="0">
+        <v>0.0011182009261601678</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
@@ -760,6 +1014,12 @@
       <c r="J14" s="0">
         <v>1.5956381144965098e-05</v>
       </c>
+      <c r="K14" s="0">
+        <v>4.7865752909640882e-10</v>
+      </c>
+      <c r="L14" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
@@ -792,6 +1052,12 @@
       <c r="J15" s="0">
         <v>3.344096327939648e-05</v>
       </c>
+      <c r="K15" s="0">
+        <v>6.8997580300650378e-10</v>
+      </c>
+      <c r="L15" s="0">
+        <v>0.0026729973766558882</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
@@ -824,6 +1090,12 @@
       <c r="J16" s="0">
         <v>4.1673745869787373e-05</v>
       </c>
+      <c r="K16" s="0">
+        <v>3.9667137478237872e-10</v>
+      </c>
+      <c r="L16" s="0">
+        <v>0.0026662461161901982</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
@@ -856,6 +1128,12 @@
       <c r="J17" s="0">
         <v>8.7913412781685647e-05</v>
       </c>
+      <c r="K17" s="0">
+        <v>3.8935433669503122e-09</v>
+      </c>
+      <c r="L17" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
@@ -888,6 +1166,12 @@
       <c r="J18" s="0">
         <v>9.5639754895881608e-06</v>
       </c>
+      <c r="K18" s="0">
+        <v>3.9055154028884649e-11</v>
+      </c>
+      <c r="L18" s="0">
+        <v>0.0011376232556794992</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
@@ -920,6 +1204,12 @@
       <c r="J19" s="0">
         <v>5.2742133689405931e-05</v>
       </c>
+      <c r="K19" s="0">
+        <v>5.5517606179910539e-10</v>
+      </c>
+      <c r="L19" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
@@ -952,6 +1242,12 @@
       <c r="J20" s="0">
         <v>3.9531435728995255e-05</v>
       </c>
+      <c r="K20" s="0">
+        <v>3.3037784021515557e-10</v>
+      </c>
+      <c r="L20" s="0">
+        <v>0.00036875223203941901</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
@@ -984,6 +1280,12 @@
       <c r="J21" s="0">
         <v>8.8891340800882564e-05</v>
       </c>
+      <c r="K21" s="0">
+        <v>6.4490798400979683e-09</v>
+      </c>
+      <c r="L21" s="0">
+        <v>0.00075685492202894023</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
@@ -1016,6 +1318,12 @@
       <c r="J22" s="0">
         <v>8.2093545618242947e-06</v>
       </c>
+      <c r="K22" s="0">
+        <v>3.6898998321109322e-10</v>
+      </c>
+      <c r="L22" s="0">
+        <v>0.0018549894420872219</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
@@ -1048,6 +1356,12 @@
       <c r="J23" s="0">
         <v>8.2376694516012987e-06</v>
       </c>
+      <c r="K23" s="0">
+        <v>5.8859993192394664e-10</v>
+      </c>
+      <c r="L23" s="0">
+        <v>0.0030598839865406428</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
@@ -1080,6 +1394,12 @@
       <c r="J24" s="0">
         <v>5.094274442183227e-05</v>
       </c>
+      <c r="K24" s="0">
+        <v>1.1054737401524598e-10</v>
+      </c>
+      <c r="L24" s="0">
+        <v>0.0017138874773836915</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
@@ -1112,6 +1432,12 @@
       <c r="J25" s="0">
         <v>8.6147097390144953e-05</v>
       </c>
+      <c r="K25" s="0">
+        <v>1.7359692305158363e-09</v>
+      </c>
+      <c r="L25" s="0">
+        <v>0.00052183941707788575</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
@@ -1144,6 +1470,12 @@
       <c r="J26" s="0">
         <v>3.0666288084672566e-05</v>
       </c>
+      <c r="K26" s="0">
+        <v>7.7612331276622276e-11</v>
+      </c>
+      <c r="L26" s="0">
+        <v>0.00013975023343523049</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
@@ -1176,6 +1508,12 @@
       <c r="J27" s="0">
         <v>4.957182077218877e-05</v>
       </c>
+      <c r="K27" s="0">
+        <v>3.3063743518524995e-10</v>
+      </c>
+      <c r="L27" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
@@ -1208,6 +1546,12 @@
       <c r="J28" s="0">
         <v>6.2008780729210604e-05</v>
       </c>
+      <c r="K28" s="0">
+        <v>3.242229031455656e-11</v>
+      </c>
+      <c r="L28" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
@@ -1240,6 +1584,12 @@
       <c r="J29" s="0">
         <v>2.5844800619842167e-05</v>
       </c>
+      <c r="K29" s="0">
+        <v>1.3649292687115277e-10</v>
+      </c>
+      <c r="L29" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
@@ -1272,6 +1622,12 @@
       <c r="J30" s="0">
         <v>2.6417246109338537e-05</v>
       </c>
+      <c r="K30" s="0">
+        <v>1.2331940469503418e-10</v>
+      </c>
+      <c r="L30" s="0">
+        <v>0.00077818166458418203</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
@@ -1304,6 +1660,12 @@
       <c r="J31" s="0">
         <v>4.7867122317589869e-05</v>
       </c>
+      <c r="K31" s="0">
+        <v>2.32370276376387e-10</v>
+      </c>
+      <c r="L31" s="0">
+        <v>0.002541386154732143</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
@@ -1336,6 +1698,12 @@
       <c r="J32" s="0">
         <v>3.1585320054412819e-05</v>
       </c>
+      <c r="K32" s="0">
+        <v>5.3245454144285571e-10</v>
+      </c>
+      <c r="L32" s="0">
+        <v>0.0012327456654148109</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
@@ -1368,6 +1736,12 @@
       <c r="J33" s="0">
         <v>1.6815314405844317e-05</v>
       </c>
+      <c r="K33" s="0">
+        <v>6.0822767198504626e-10</v>
+      </c>
+      <c r="L33" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
@@ -1400,6 +1774,12 @@
       <c r="J34" s="0">
         <v>9.3348945642611787e-06</v>
       </c>
+      <c r="K34" s="0">
+        <v>1.8035242637837484e-10</v>
+      </c>
+      <c r="L34" s="0">
+        <v>0.0009104791784758971</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
@@ -1432,6 +1812,12 @@
       <c r="J35" s="0">
         <v>3.0605989774885914e-05</v>
       </c>
+      <c r="K35" s="0">
+        <v>2.7626809141815622e-10</v>
+      </c>
+      <c r="L35" s="0">
+        <v>0.00052861626848436699</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
@@ -1464,6 +1850,12 @@
       <c r="J36" s="0">
         <v>3.8162835068901945e-05</v>
       </c>
+      <c r="K36" s="0">
+        <v>5.9282465228610497e-10</v>
+      </c>
+      <c r="L36" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
@@ -1496,6 +1888,12 @@
       <c r="J37" s="0">
         <v>2.6281562769424877e-05</v>
       </c>
+      <c r="K37" s="0">
+        <v>8.7745168391959801e-11</v>
+      </c>
+      <c r="L37" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
@@ -1528,6 +1926,12 @@
       <c r="J38" s="0">
         <v>6.1623473789142374e-06</v>
       </c>
+      <c r="K38" s="0">
+        <v>3.1707708768868518e-10</v>
+      </c>
+      <c r="L38" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
@@ -1560,6 +1964,12 @@
       <c r="J39" s="0">
         <v>4.3693550358864862e-05</v>
       </c>
+      <c r="K39" s="0">
+        <v>3.5624489733570043e-10</v>
+      </c>
+      <c r="L39" s="0">
+        <v>0.00085636162829489943</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
@@ -1592,6 +2002,12 @@
       <c r="J40" s="0">
         <v>4.0348246900005466e-05</v>
       </c>
+      <c r="K40" s="0">
+        <v>2.9262953184868764e-10</v>
+      </c>
+      <c r="L40" s="0">
+        <v>0.0019312998079580857</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
@@ -1624,6 +2040,12 @@
       <c r="J41" s="0">
         <v>3.9550784520525257e-05</v>
       </c>
+      <c r="K41" s="0">
+        <v>3.5471020879492147e-10</v>
+      </c>
+      <c r="L41" s="0">
+        <v>0.0011054317685990501</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
@@ -1656,6 +2078,12 @@
       <c r="J42" s="0">
         <v>2.0591897841745639e-05</v>
       </c>
+      <c r="K42" s="0">
+        <v>1.1096276154166575e-10</v>
+      </c>
+      <c r="L42" s="0">
+        <v>0.00081182672711400342</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
@@ -1688,6 +2116,12 @@
       <c r="J43" s="0">
         <v>8.2843549008006546e-06</v>
       </c>
+      <c r="K43" s="0">
+        <v>3.7668437371279533e-10</v>
+      </c>
+      <c r="L43" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
@@ -1720,6 +2154,12 @@
       <c r="J44" s="0">
         <v>4.7708879020690124e-05</v>
       </c>
+      <c r="K44" s="0">
+        <v>3.4486502920637449e-10</v>
+      </c>
+      <c r="L44" s="0">
+        <v>0.0013933754493322659</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
@@ -1752,6 +2192,12 @@
       <c r="J45" s="0">
         <v>1.6082477277418392e-05</v>
       </c>
+      <c r="K45" s="0">
+        <v>1.2895939576608343e-11</v>
+      </c>
+      <c r="L45" s="0">
+        <v>0.00057297169540637726</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
@@ -1784,6 +2230,12 @@
       <c r="J46" s="0">
         <v>2.8697235642444996e-05</v>
       </c>
+      <c r="K46" s="0">
+        <v>1.2332428554670161e-10</v>
+      </c>
+      <c r="L46" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
@@ -1816,6 +2268,12 @@
       <c r="J47" s="0">
         <v>2.6074781165241201e-05</v>
       </c>
+      <c r="K47" s="0">
+        <v>1.1050960671588819e-10</v>
+      </c>
+      <c r="L47" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
@@ -1848,6 +2306,12 @@
       <c r="J48" s="0">
         <v>2.8788320744152103e-05</v>
       </c>
+      <c r="K48" s="0">
+        <v>6.2914883628861042e-10</v>
+      </c>
+      <c r="L48" s="0">
+        <v>0.0010132175256538371</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
@@ -1880,6 +2344,12 @@
       <c r="J49" s="0">
         <v>6.652795587312899e-05</v>
       </c>
+      <c r="K49" s="0">
+        <v>5.7479155814433513e-10</v>
+      </c>
+      <c r="L49" s="0">
+        <v>0.00035261245954343367</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="0">
@@ -1912,6 +2382,12 @@
       <c r="J50" s="0">
         <v>1.9985084066088434e-05</v>
       </c>
+      <c r="K50" s="0">
+        <v>2.3591663440477376e-10</v>
+      </c>
+      <c r="L50" s="0">
+        <v>0.001009854639767742</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="0">
@@ -1944,6 +2420,12 @@
       <c r="J51" s="0">
         <v>4.32361704375614e-05</v>
       </c>
+      <c r="K51" s="0">
+        <v>1.6952553185586224e-10</v>
+      </c>
+      <c r="L51" s="0">
+        <v>0.00090625872731556103</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="0">
@@ -1976,6 +2458,12 @@
       <c r="J52" s="0">
         <v>5.0408033418964457e-05</v>
       </c>
+      <c r="K52" s="0">
+        <v>4.6862309223483956e-10</v>
+      </c>
+      <c r="L52" s="0">
+        <v>0.0020660583177249882</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="0">
@@ -2008,6 +2496,12 @@
       <c r="J53" s="0">
         <v>2.2739444312186381e-05</v>
       </c>
+      <c r="K53" s="0">
+        <v>2.230906981728639e-10</v>
+      </c>
+      <c r="L53" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="0">
@@ -2040,6 +2534,12 @@
       <c r="J54" s="0">
         <v>1.9188701362595636e-05</v>
       </c>
+      <c r="K54" s="0">
+        <v>6.0543531376507057e-10</v>
+      </c>
+      <c r="L54" s="0">
+        <v>0.001586945785572788</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="0">
@@ -2072,6 +2572,12 @@
       <c r="J55" s="0">
         <v>3.8392036820424193e-05</v>
       </c>
+      <c r="K55" s="0">
+        <v>4.904018638463307e-10</v>
+      </c>
+      <c r="L55" s="0">
+        <v>0.0030479640223355993</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="0">
@@ -2104,6 +2610,12 @@
       <c r="J56" s="0">
         <v>2.0471695931641034e-05</v>
       </c>
+      <c r="K56" s="0">
+        <v>1.9594762663465729e-10</v>
+      </c>
+      <c r="L56" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="0">
@@ -2136,6 +2648,12 @@
       <c r="J57" s="0">
         <v>9.4409220768612332e-06</v>
       </c>
+      <c r="K57" s="0">
+        <v>1.4663071557502476e-10</v>
+      </c>
+      <c r="L57" s="0">
+        <v>0.0024096514808381541</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="0">
@@ -2168,6 +2686,12 @@
       <c r="J58" s="0">
         <v>3.6887589360519556e-05</v>
       </c>
+      <c r="K58" s="0">
+        <v>1.0867312690047804e-10</v>
+      </c>
+      <c r="L58" s="0">
+        <v>0.00055715231537664721</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="0">
@@ -2200,6 +2724,12 @@
       <c r="J59" s="0">
         <v>1.5471473736881515e-05</v>
       </c>
+      <c r="K59" s="0">
+        <v>7.674857766456809e-11</v>
+      </c>
+      <c r="L59" s="0">
+        <v>0.00052788099439227772</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="0">
@@ -2232,6 +2762,12 @@
       <c r="J60" s="0">
         <v>3.332953329016989e-05</v>
       </c>
+      <c r="K60" s="0">
+        <v>6.9100666596097346e-10</v>
+      </c>
+      <c r="L60" s="0">
+        <v>0.0024285129360638144</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="0">
@@ -2264,6 +2800,12 @@
       <c r="J61" s="0">
         <v>6.8874467209419459e-05</v>
       </c>
+      <c r="K61" s="0">
+        <v>2.5372461027941958e-10</v>
+      </c>
+      <c r="L61" s="0">
+        <v>0.0010474374087166942</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="0">
@@ -2296,6 +2838,12 @@
       <c r="J62" s="0">
         <v>1.5363070332570753e-05</v>
       </c>
+      <c r="K62" s="0">
+        <v>2.9328808368792216e-10</v>
+      </c>
+      <c r="L62" s="0">
+        <v>0.0011718893963331332</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="0">
@@ -2328,6 +2876,12 @@
       <c r="J63" s="0">
         <v>1.3072287151249743e-05</v>
       </c>
+      <c r="K63" s="0">
+        <v>4.3687681063310564e-10</v>
+      </c>
+      <c r="L63" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="0">
@@ -2360,6 +2914,12 @@
       <c r="J64" s="0">
         <v>3.5219087151014517e-05</v>
       </c>
+      <c r="K64" s="0">
+        <v>2.7915508637361924e-11</v>
+      </c>
+      <c r="L64" s="0">
+        <v>0.00037193131949005294</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="0">
@@ -2392,6 +2952,12 @@
       <c r="J65" s="0">
         <v>8.4936235926790048e-06</v>
       </c>
+      <c r="K65" s="0">
+        <v>3.4308637211652721e-10</v>
+      </c>
+      <c r="L65" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="0">
@@ -2424,6 +2990,12 @@
       <c r="J66" s="0">
         <v>1.1596602635062722e-05</v>
       </c>
+      <c r="K66" s="0">
+        <v>9.8705585023034232e-11</v>
+      </c>
+      <c r="L66" s="0">
+        <v>0.0013803708691033612</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="0">
@@ -2456,6 +3028,12 @@
       <c r="J67" s="0">
         <v>2.0920589309682819e-05</v>
       </c>
+      <c r="K67" s="0">
+        <v>2.4517127570102066e-10</v>
+      </c>
+      <c r="L67" s="0">
+        <v>0.0010804602993190738</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="0">
@@ -2488,6 +3066,12 @@
       <c r="J68" s="0">
         <v>4.2099719461148262e-05</v>
       </c>
+      <c r="K68" s="0">
+        <v>1.1251554722723348e-11</v>
+      </c>
+      <c r="L68" s="0">
+        <v>0.00066949886970645597</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="0">
@@ -2520,6 +3104,12 @@
       <c r="J69" s="0">
         <v>1.334793662671416e-05</v>
       </c>
+      <c r="K69" s="0">
+        <v>2.064023528449614e-10</v>
+      </c>
+      <c r="L69" s="0">
+        <v>0.00083811230750714541</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="0">
@@ -2552,6 +3142,12 @@
       <c r="J70" s="0">
         <v>5.3739843641989372e-05</v>
       </c>
+      <c r="K70" s="0">
+        <v>8.6717641598387587e-11</v>
+      </c>
+      <c r="L70" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="0">
@@ -2584,6 +3180,12 @@
       <c r="J71" s="0">
         <v>1.9205362444332698e-05</v>
       </c>
+      <c r="K71" s="0">
+        <v>3.729899109302348e-11</v>
+      </c>
+      <c r="L71" s="0">
+        <v>0.0014217435911313301</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="0">
@@ -2616,6 +3218,12 @@
       <c r="J72" s="0">
         <v>3.1203740127672893e-05</v>
       </c>
+      <c r="K72" s="0">
+        <v>2.0022932154771685e-10</v>
+      </c>
+      <c r="L72" s="0">
+        <v>0.0013240364922897309</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="0">
@@ -2648,6 +3256,12 @@
       <c r="J73" s="0">
         <v>8.6071923817279077e-06</v>
       </c>
+      <c r="K73" s="0">
+        <v>2.5245324186517389e-10</v>
+      </c>
+      <c r="L73" s="0">
+        <v>0.0015669851967871171</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="0">
@@ -2680,6 +3294,12 @@
       <c r="J74" s="0">
         <v>2.5925743764835317e-05</v>
       </c>
+      <c r="K74" s="0">
+        <v>1.5481350705588212e-10</v>
+      </c>
+      <c r="L74" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="0">
@@ -2712,6 +3332,12 @@
       <c r="J75" s="0">
         <v>6.303843232111986e-06</v>
       </c>
+      <c r="K75" s="0">
+        <v>2.5794348193853554e-10</v>
+      </c>
+      <c r="L75" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="0">
@@ -2744,6 +3370,12 @@
       <c r="J76" s="0">
         <v>5.1344270095968264e-05</v>
       </c>
+      <c r="K76" s="0">
+        <v>3.8833122328035974e-11</v>
+      </c>
+      <c r="L76" s="0">
+        <v>0.00048474922135848295</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="0">
@@ -2776,6 +3408,12 @@
       <c r="J77" s="0">
         <v>2.5357579137182399e-05</v>
       </c>
+      <c r="K77" s="0">
+        <v>4.9272433594169906e-11</v>
+      </c>
+      <c r="L77" s="0">
+        <v>0.00066227378257037201</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="0">
@@ -2808,6 +3446,12 @@
       <c r="J78" s="0">
         <v>4.891102681316482e-05</v>
       </c>
+      <c r="K78" s="0">
+        <v>2.7974490576251631e-11</v>
+      </c>
+      <c r="L78" s="0">
+        <v>0.00097175908799298561</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="0">
@@ -2840,6 +3484,12 @@
       <c r="J79" s="0">
         <v>3.0917536780087185e-05</v>
       </c>
+      <c r="K79" s="0">
+        <v>2.1079546684517547e-11</v>
+      </c>
+      <c r="L79" s="0">
+        <v>0.0015154521226467292</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="0">
@@ -2872,6 +3522,12 @@
       <c r="J80" s="0">
         <v>2.4965857194671787e-05</v>
       </c>
+      <c r="K80" s="0">
+        <v>6.0831956581429353e-11</v>
+      </c>
+      <c r="L80" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="0">
@@ -2904,6 +3560,12 @@
       <c r="J81" s="0">
         <v>2.4908715093218983e-05</v>
       </c>
+      <c r="K81" s="0">
+        <v>2.039141134817225e-08</v>
+      </c>
+      <c r="L81" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="0">
@@ -2936,6 +3598,12 @@
       <c r="J82" s="0">
         <v>2.257381797855729e-05</v>
       </c>
+      <c r="K82" s="0">
+        <v>9.8018712137061935e-10</v>
+      </c>
+      <c r="L82" s="0">
+        <v>0.003543900305144346</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="0">
@@ -2968,6 +3636,12 @@
       <c r="J83" s="0">
         <v>5.470884101584741e-05</v>
       </c>
+      <c r="K83" s="0">
+        <v>9.3921177689324965e-11</v>
+      </c>
+      <c r="L83" s="0">
+        <v>0.0014777039592767673</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="0">
@@ -3000,6 +3674,12 @@
       <c r="J84" s="0">
         <v>5.5550850235681598e-05</v>
       </c>
+      <c r="K84" s="0">
+        <v>5.0757244257402089e-10</v>
+      </c>
+      <c r="L84" s="0">
+        <v>0.0002812442308026135</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="0">
@@ -3032,6 +3712,12 @@
       <c r="J85" s="0">
         <v>7.2571456951412646e-06</v>
       </c>
+      <c r="K85" s="0">
+        <v>5.5622132049780105e-11</v>
+      </c>
+      <c r="L85" s="0">
+        <v>0.0024871381496275441</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="0">
@@ -3064,6 +3750,12 @@
       <c r="J86" s="0">
         <v>2.2157908612065627e-05</v>
       </c>
+      <c r="K86" s="0">
+        <v>5.2004050318639779e-10</v>
+      </c>
+      <c r="L86" s="0">
+        <v>0.0020783852658178424</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="0">
@@ -3096,6 +3788,12 @@
       <c r="J87" s="0">
         <v>3.2832810302871398e-05</v>
       </c>
+      <c r="K87" s="0">
+        <v>9.5188270247418425e-11</v>
+      </c>
+      <c r="L87" s="0">
+        <v>0.0013270577971665042</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="0">
@@ -3128,6 +3826,12 @@
       <c r="J88" s="0">
         <v>8.3031684986073534e-06</v>
       </c>
+      <c r="K88" s="0">
+        <v>1.0464794425518837e-11</v>
+      </c>
+      <c r="L88" s="0">
+        <v>0.0011993030192789156</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="0">
@@ -3160,6 +3864,12 @@
       <c r="J89" s="0">
         <v>3.885067732641398e-05</v>
       </c>
+      <c r="K89" s="0">
+        <v>1.9252951523003812e-10</v>
+      </c>
+      <c r="L89" s="0">
+        <v>0.00041198420638526137</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="0">
@@ -3192,6 +3902,12 @@
       <c r="J90" s="0">
         <v>3.2673302761349842e-05</v>
       </c>
+      <c r="K90" s="0">
+        <v>4.7549801894939473e-10</v>
+      </c>
+      <c r="L90" s="0">
+        <v>0.0007505905671013446</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="0">
@@ -3224,6 +3940,12 @@
       <c r="J91" s="0">
         <v>4.9157963192517326e-05</v>
       </c>
+      <c r="K91" s="0">
+        <v>8.3823978131542226e-11</v>
+      </c>
+      <c r="L91" s="0">
+        <v>0.00019565014244802312</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="0">
@@ -3256,6 +3978,12 @@
       <c r="J92" s="0">
         <v>1.6408580963597037e-05</v>
       </c>
+      <c r="K92" s="0">
+        <v>1.9705349751499673e-10</v>
+      </c>
+      <c r="L92" s="0">
+        <v>0.0028959839501388421</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="0">
@@ -3288,6 +4016,12 @@
       <c r="J93" s="0">
         <v>8.4887949718428089e-05</v>
       </c>
+      <c r="K93" s="0">
+        <v>2.6972072725787432e-10</v>
+      </c>
+      <c r="L93" s="0">
+        <v>0.00044422816010053403</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="0">
@@ -3320,6 +4054,12 @@
       <c r="J94" s="0">
         <v>2.7173438753176957e-05</v>
       </c>
+      <c r="K94" s="0">
+        <v>3.0863832181971891e-10</v>
+      </c>
+      <c r="L94" s="0">
+        <v>0.00013180773767133513</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="0">
@@ -3352,6 +4092,12 @@
       <c r="J95" s="0">
         <v>2.7098170191088504e-05</v>
       </c>
+      <c r="K95" s="0">
+        <v>3.4440608898775857e-10</v>
+      </c>
+      <c r="L95" s="0">
+        <v>0.00067626025258066204</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="0">
@@ -3384,6 +4130,12 @@
       <c r="J96" s="0">
         <v>1.5185664237026237e-05</v>
       </c>
+      <c r="K96" s="0">
+        <v>4.3074052400024401e-11</v>
+      </c>
+      <c r="L96" s="0">
+        <v>0.0016727589643775382</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="0">
@@ -3416,6 +4168,12 @@
       <c r="J97" s="0">
         <v>4.9553260050897542e-05</v>
       </c>
+      <c r="K97" s="0">
+        <v>2.1835988933756278e-10</v>
+      </c>
+      <c r="L97" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="0">
@@ -3448,6 +4206,12 @@
       <c r="J98" s="0">
         <v>5.001680353952883e-05</v>
       </c>
+      <c r="K98" s="0">
+        <v>2.8142226588592903e-11</v>
+      </c>
+      <c r="L98" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="0">
@@ -3480,6 +4244,12 @@
       <c r="J99" s="0">
         <v>4.6146004504259944e-06</v>
       </c>
+      <c r="K99" s="0">
+        <v>1.0044667634010858e-10</v>
+      </c>
+      <c r="L99" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="0">
@@ -3512,6 +4282,12 @@
       <c r="J100" s="0">
         <v>4.2452871271004948e-05</v>
       </c>
+      <c r="K100" s="0">
+        <v>9.0966722397520738e-11</v>
+      </c>
+      <c r="L100" s="0">
+        <v>0.00027971255917133927</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="0">
@@ -3544,6 +4320,12 @@
       <c r="J101" s="0">
         <v>3.9120663959426242e-05</v>
       </c>
+      <c r="K101" s="0">
+        <v>8.7624709429592982e-11</v>
+      </c>
+      <c r="L101" s="0">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>